<commit_message>
Trying to get the table insert into DB
</commit_message>
<xml_diff>
--- a/result_table_templates/SAHP.xlsx
+++ b/result_table_templates/SAHP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\MATLAB\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0808FDB-48F1-42F3-B539-55466ACA74C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432B29F-CE50-403E-BE97-B2ECC1F0D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,12 +179,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -210,9 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +537,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +551,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -732,7 +739,7 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -743,7 +750,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>

</xml_diff>